<commit_message>
made the view panel for the data.
</commit_message>
<xml_diff>
--- a/Templates/Data/Unames2.xlsx
+++ b/Templates/Data/Unames2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="42" uniqueCount="7">
   <si>
     <t>Created by LibXL trial version 4.6.0. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -91,7 +91,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV3"/>
+  <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -380,20 +380,117 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" t="s">
+    <row r="4">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made delete easy for the file
</commit_message>
<xml_diff>
--- a/Templates/Data/Unames2.xlsx
+++ b/Templates/Data/Unames2.xlsx
@@ -14,27 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="42" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1" uniqueCount="1">
   <si>
     <t>Created by LibXL trial version 4.6.0. Please buy the LibXL full version for removing this message.</t>
-  </si>
-  <si>
-    <t>toggle</t>
-  </si>
-  <si>
-    <t>radio</t>
-  </si>
-  <si>
-    <t>dropdown</t>
-  </si>
-  <si>
-    <t>checkbox</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -91,7 +73,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
+  <dimension ref="A1:IV1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -357,143 +339,6 @@
       <c r="IU1" s="1"/>
       <c r="IV1" s="1"/>
     </row>
-    <row r="2">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:IV1"/>

</xml_diff>